<commit_message>
03.04 - Task05-2 Select Rows Number
</commit_message>
<xml_diff>
--- a/test_case_olusturma_sablonu.xlsx
+++ b/test_case_olusturma_sablonu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" activeTab="1"/>
+    <workbookView windowWidth="13755" windowHeight="12225" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
   <si>
     <t>project name</t>
   </si>
@@ -246,11 +246,6 @@
     <t>Get text of any cell</t>
   </si>
   <si>
-    <t xml:space="preserve">1.Navigate to Web Site
-3.Go to Web Tables in Elements
-</t>
-  </si>
-  <si>
     <t>1.Get text from "Kierra" 's email
 2.Verify that the text you get equals "cierra@example.com
 "</t>
@@ -265,6 +260,49 @@
   </si>
   <si>
     <t>Successfull</t>
+  </si>
+  <si>
+    <t>TS_WT_002</t>
+  </si>
+  <si>
+    <t>Select Rows and Previous and Next Buttons</t>
+  </si>
+  <si>
+    <t>TC_WT_SelectRows_001</t>
+  </si>
+  <si>
+    <t>Select number of lines  for a page</t>
+  </si>
+  <si>
+    <t>1. Ad 10 new rows by JavaFaker
+2. Select 5 rows for a page
+3. verify that there are 5 rows on the page</t>
+  </si>
+  <si>
+    <t>rows : JavaFaker
+expectedNumberOfRows: 5</t>
+  </si>
+  <si>
+    <t>expectedNumberOfRows: 5</t>
+  </si>
+  <si>
+    <t>TC_WT_SelectRows_002</t>
+  </si>
+  <si>
+    <t>Check Previous and Next Buttons Functionality</t>
+  </si>
+  <si>
+    <t>1.Verify that Previous and Next Buttons are unclickable
+2. Ad 10 new rows
+3. Select 5 rows for a page
+4. Verify that Previous Button is unclickable and Nextt Button is clickable
+5.Click Next Button
+6.Verify that Previous Button is clickable and Nextt Button is unclickable</t>
+  </si>
+  <si>
+    <t>step1: P-&gt; unclickable, N-&gt; unclickable
+step3: P-&gt; unclickable, N-&gt; clickable
+step5: P-&gt; clickable, N-&gt; unclickable</t>
   </si>
 </sst>
 </file>
@@ -272,10 +310,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -289,6 +327,29 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -300,8 +361,71 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,7 +440,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,112 +468,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -446,187 +484,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,26 +680,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -708,180 +744,182 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1465,10 +1503,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1478,10 +1516,10 @@
     <col min="3" max="3" width="25" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1"/>
+    <col min="6" max="6" width="39.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.25" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.3333333333333" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.3333333333333" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.8333333333333" style="1"/>
     <col min="12" max="12" width="12.6666666666667" style="1" customWidth="1"/>
@@ -1625,7 +1663,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" ht="126" spans="3:14">
+    <row r="11" ht="110.25" spans="3:14">
       <c r="C11" s="1" t="s">
         <v>62</v>
       </c>
@@ -1660,7 +1698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" ht="110.25" spans="3:13">
+    <row r="12" ht="110.25" spans="3:14">
       <c r="C12" s="1" t="s">
         <v>68</v>
       </c>
@@ -1668,28 +1706,107 @@
         <v>69</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M12" s="2">
         <v>45017</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" ht="110.25" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="2">
+        <v>45019</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" ht="141.75" spans="3:14">
+      <c r="C14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="2">
+        <v>45019</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>